<commit_message>
scout club text version
</commit_message>
<xml_diff>
--- a/tourneysps.xlsx
+++ b/tourneysps.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhengyangliu/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhengyangliu/Desktop/NFSBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF56A8A8-0D6E-6144-B3A8-D4DCB1146C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58C7A17-9461-7548-81F3-0F66DFBEC065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8089,9 +8089,6 @@
     <t>Club_Name</t>
   </si>
   <si>
-    <t>roc.no_1</t>
-  </si>
-  <si>
     <t>NeedForSpeed</t>
   </si>
   <si>
@@ -8108,6 +8105,9 @@
   </si>
   <si>
     <t>toodankfast</t>
+  </si>
+  <si>
+    <t>roc_no.1</t>
   </si>
 </sst>
 </file>
@@ -8501,8 +8501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1017"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A406" workbookViewId="0">
-      <selection activeCell="G488" sqref="G488"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9789,7 +9789,7 @@
         <v>322</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>2688</v>
+        <v>2694</v>
       </c>
       <c r="H54" s="9"/>
     </row>
@@ -12919,7 +12919,7 @@
         <v>1088</v>
       </c>
       <c r="G187" s="6" t="s">
-        <v>2689</v>
+        <v>2688</v>
       </c>
       <c r="H187" s="7"/>
     </row>
@@ -17097,7 +17097,7 @@
         <v>1085</v>
       </c>
       <c r="G365" s="6" t="s">
-        <v>2690</v>
+        <v>2689</v>
       </c>
       <c r="H365" s="11"/>
     </row>
@@ -17949,7 +17949,7 @@
         <v>2242</v>
       </c>
       <c r="G402" s="6" t="s">
-        <v>2690</v>
+        <v>2689</v>
       </c>
       <c r="H402" s="11"/>
     </row>
@@ -18088,7 +18088,7 @@
         <v>2276</v>
       </c>
       <c r="G408" s="6" t="s">
-        <v>2690</v>
+        <v>2689</v>
       </c>
       <c r="H408" s="11"/>
     </row>
@@ -18135,7 +18135,7 @@
         <v>2288</v>
       </c>
       <c r="G410" s="6" t="s">
-        <v>2690</v>
+        <v>2689</v>
       </c>
       <c r="H410" s="11"/>
     </row>
@@ -18159,7 +18159,7 @@
         <v>2294</v>
       </c>
       <c r="G411" s="6" t="s">
-        <v>2690</v>
+        <v>2689</v>
       </c>
       <c r="H411" s="11"/>
     </row>
@@ -18413,7 +18413,7 @@
         <v>2355</v>
       </c>
       <c r="G422" s="6" t="s">
-        <v>2691</v>
+        <v>2690</v>
       </c>
       <c r="H422" s="7"/>
     </row>
@@ -18509,7 +18509,7 @@
         <v>2375</v>
       </c>
       <c r="G426" s="6" t="s">
-        <v>2692</v>
+        <v>2691</v>
       </c>
       <c r="H426" s="7"/>
     </row>
@@ -18533,7 +18533,7 @@
         <v>2380</v>
       </c>
       <c r="G427" s="6" t="s">
-        <v>2693</v>
+        <v>2692</v>
       </c>
       <c r="H427" s="7"/>
     </row>
@@ -18557,7 +18557,7 @@
         <v>2386</v>
       </c>
       <c r="G428" s="6" t="s">
-        <v>2693</v>
+        <v>2692</v>
       </c>
       <c r="H428" s="7"/>
     </row>
@@ -18581,7 +18581,7 @@
         <v>2392</v>
       </c>
       <c r="G429" s="6" t="s">
-        <v>2694</v>
+        <v>2693</v>
       </c>
       <c r="H429" s="7"/>
     </row>
@@ -18653,7 +18653,7 @@
         <v>472</v>
       </c>
       <c r="G432" s="6" t="s">
-        <v>2692</v>
+        <v>2691</v>
       </c>
       <c r="H432" s="7"/>
     </row>
@@ -18773,7 +18773,7 @@
         <v>2431</v>
       </c>
       <c r="G437" s="6" t="s">
-        <v>2692</v>
+        <v>2691</v>
       </c>
       <c r="H437" s="7"/>
     </row>
@@ -18797,7 +18797,7 @@
         <v>2437</v>
       </c>
       <c r="G438" s="6" t="s">
-        <v>2692</v>
+        <v>2691</v>
       </c>
       <c r="H438" s="7"/>
     </row>

</xml_diff>